<commit_message>
Worked on Ball to player Collision
</commit_message>
<xml_diff>
--- a/TimeSheets/Time Log template_SeniorProject.xlsx
+++ b/TimeSheets/Time Log template_SeniorProject.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>Added BreakOut Scene, Added Player Movement for BreakOut, Assets, and BallControl:BreakOut (unfinished)</t>
+  </si>
+  <si>
+    <t>11:20am</t>
+  </si>
+  <si>
+    <t>Worked on BreakOut Collision Ball and Player</t>
   </si>
 </sst>
 </file>
@@ -645,12 +651,24 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="5"/>
+      <c r="A7" s="2">
+        <v>41933</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="6">
+        <v>140</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>

</xml_diff>

<commit_message>
Completed basic mechanics of ball and player, added brick data.
</commit_message>
<xml_diff>
--- a/TimeSheets/Time Log template_SeniorProject.xlsx
+++ b/TimeSheets/Time Log template_SeniorProject.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -97,6 +97,33 @@
   </si>
   <si>
     <t>Worked on BreakOut Collision Ball and Player</t>
+  </si>
+  <si>
+    <t>2:00am</t>
+  </si>
+  <si>
+    <t>5:00am</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>2 hours 30</t>
+  </si>
+  <si>
+    <t>4 hours 10</t>
+  </si>
+  <si>
+    <t>4 hours</t>
+  </si>
+  <si>
+    <t>3 hours 20</t>
+  </si>
+  <si>
+    <t>Compelted basic mechancs of ball and player, added brick data.</t>
   </si>
 </sst>
 </file>
@@ -185,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -216,6 +243,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -524,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,22 +565,24 @@
     <col min="1" max="1" width="8.28515625" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="58.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-    </row>
-    <row r="2" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -561,16 +593,19 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>41885</v>
       </c>
@@ -580,17 +615,20 @@
       <c r="C3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="10">
         <v>90</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>41906</v>
       </c>
@@ -600,17 +638,20 @@
       <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="6">
         <v>130</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>41907</v>
       </c>
@@ -620,17 +661,20 @@
       <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="6">
         <v>250</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>41928</v>
       </c>
@@ -640,17 +684,20 @@
       <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="6">
         <v>220</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>41933</v>
       </c>
@@ -660,198 +707,237 @@
       <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="6">
         <v>140</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="F7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>41935</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="6">
+        <v>180</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="3"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="3"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="3"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="3"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="3"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="3"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="3"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="3"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="3"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="3"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="3"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="3"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="3"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="3"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="3"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="3"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="3"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="5"/>
-    </row>
-    <row r="27" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="3"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="5"/>
-    </row>
-    <row r="28" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="3"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="3"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="5"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F29">
       <formula1>"Website, Documentation, Research, Programming, GUI, Marketing, Site Details,Code Details"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
tried for color change upon collision
</commit_message>
<xml_diff>
--- a/TimeSheets/Time Log template_SeniorProject.xlsx
+++ b/TimeSheets/Time Log template_SeniorProject.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KG3UNFORGN\Documents\KalebSeniorProject\TimeSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaleb\Documents\KalebSeniorProject\TimeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>TOTAL HOURS:</t>
+  </si>
+  <si>
+    <t>Tried changing block color upon collision</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>Researched how detect collision between two objects</t>
   </si>
 </sst>
 </file>
@@ -202,17 +211,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,15 +545,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -579,10 +588,10 @@
       <c r="C3" s="9">
         <v>0.94444444444444453</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="12">
         <v>1</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="12">
         <v>90</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -731,54 +740,82 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="5"/>
+      <c r="A10" s="2">
+        <v>41948</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D10" s="6">
+        <v>3</v>
+      </c>
+      <c r="E10" s="6">
+        <v>180</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="5"/>
+      <c r="A11" s="2">
+        <v>41948</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6">
+        <v>110</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="6">
-        <f>SUM(E3:E9)</f>
-        <v>1200</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="4"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="6">
+        <f>SUM(E5:E11)</f>
+        <v>1270</v>
+      </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="5"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -915,12 +952,30 @@
       <c r="F29" s="4"/>
       <c r="G29" s="5"/>
     </row>
+    <row r="30" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F31">
       <formula1>"Website, Documentation, Research, Programming, GUI, Marketing, Site Details,Code Details"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>